<commit_message>
Re-organisation dossier + ajout partie HW
J'ai ajouter la partie HW avec des fichier de CAO et des shema
Il y a aussi un fichier "Table des matieres" qui contiens une organisation generale du rapport il est a detailler
</commit_message>
<xml_diff>
--- a/Documentation Software/DefinitionTrame -Sonia.xlsx
+++ b/Documentation Software/DefinitionTrame -Sonia.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/Polytech_EII_3/Projet Elec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Gateway_py\Documentation Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1680" windowWidth="25540" windowHeight="16360"/>
+    <workbookView xWindow="675" yWindow="1680" windowWidth="25545" windowHeight="16365" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format trame et requete PHP" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Définition trame Station" sheetId="1" r:id="rId3"/>
     <sheet name="Définition trame Ruche" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -311,8 +311,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1458,45 +1458,75 @@
     <xf numFmtId="49" fontId="15" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1505,36 +1535,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2694,74 +2694,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView topLeftCell="A3" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="2.5" style="51" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="51" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="29" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="51" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="51" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
-    <col min="16" max="16" width="2.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="2.6640625" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="20" width="2.6640625" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" customWidth="1"/>
-    <col min="22" max="22" width="2.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="1.1640625" style="51" customWidth="1"/>
-    <col min="25" max="30" width="10.6640625" style="51" customWidth="1"/>
-    <col min="31" max="32" width="10.83203125" style="51"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="1.140625" style="51" customWidth="1"/>
+    <col min="25" max="30" width="10.7109375" style="51" customWidth="1"/>
+    <col min="31" max="32" width="10.85546875" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" s="51" customFormat="1">
       <c r="D1" s="53"/>
     </row>
-    <row r="2" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:32" s="51" customFormat="1">
       <c r="D2" s="53"/>
     </row>
-    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.15">
-      <c r="D3" s="107" t="s">
+    <row r="3" spans="1:32" ht="18">
+      <c r="D3" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-    </row>
-    <row r="4" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+    </row>
+    <row r="4" spans="1:32" s="51" customFormat="1">
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="57"/>
@@ -2769,7 +2769,7 @@
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
     </row>
-    <row r="5" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:32" s="51" customFormat="1">
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="57"/>
@@ -2791,38 +2791,38 @@
       <c r="W5" s="63"/>
       <c r="X5" s="64"/>
     </row>
-    <row r="6" spans="1:32" s="122" customFormat="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="123"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="F6" s="122" t="s">
+    <row r="6" spans="1:32" s="104" customFormat="1" ht="24.75" thickBot="1">
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="F6" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="124"/>
-      <c r="I6" s="123" t="s">
+      <c r="H6" s="106"/>
+      <c r="I6" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123" t="s">
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="N6" s="123"/>
-      <c r="O6" s="123" t="s">
+      <c r="N6" s="105"/>
+      <c r="O6" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="P6" s="123"/>
-      <c r="Q6" s="123"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
-      <c r="T6" s="123"/>
-      <c r="U6" s="123"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="123"/>
-      <c r="X6" s="125"/>
-    </row>
-    <row r="7" spans="1:32" s="35" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="105"/>
+      <c r="T6" s="105"/>
+      <c r="U6" s="105"/>
+      <c r="V6" s="105"/>
+      <c r="W6" s="105"/>
+      <c r="X6" s="107"/>
+    </row>
+    <row r="7" spans="1:32" s="35" customFormat="1" ht="20.25" customHeight="1">
       <c r="A7" s="52"/>
       <c r="B7" s="58"/>
       <c r="C7" s="75"/>
@@ -2836,38 +2836,38 @@
       <c r="G7" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="115" t="s">
+      <c r="H7" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="109"/>
-      <c r="J7" s="108" t="s">
+      <c r="I7" s="122"/>
+      <c r="J7" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="108" t="s">
+      <c r="K7" s="122"/>
+      <c r="L7" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="109"/>
-      <c r="N7" s="108" t="s">
+      <c r="M7" s="122"/>
+      <c r="N7" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="109"/>
-      <c r="P7" s="108" t="s">
+      <c r="O7" s="122"/>
+      <c r="P7" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="108" t="s">
+      <c r="Q7" s="122"/>
+      <c r="R7" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="S7" s="109"/>
-      <c r="T7" s="108" t="s">
+      <c r="S7" s="122"/>
+      <c r="T7" s="123" t="s">
         <v>50</v>
       </c>
-      <c r="U7" s="109"/>
-      <c r="V7" s="108" t="s">
+      <c r="U7" s="122"/>
+      <c r="V7" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="W7" s="109"/>
+      <c r="W7" s="122"/>
       <c r="X7" s="65"/>
       <c r="Y7" s="52"/>
       <c r="Z7" s="52"/>
@@ -2878,7 +2878,7 @@
       <c r="AE7" s="52"/>
       <c r="AF7" s="52"/>
     </row>
-    <row r="8" spans="1:32" s="29" customFormat="1" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" s="29" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
       <c r="A8" s="53"/>
       <c r="B8" s="57"/>
       <c r="C8" s="60"/>
@@ -2950,7 +2950,7 @@
       <c r="AE8" s="53"/>
       <c r="AF8" s="53"/>
     </row>
-    <row r="9" spans="1:32" s="51" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:32" s="51" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
       <c r="D9" s="57"/>
@@ -2975,32 +2975,32 @@
       <c r="W9" s="67"/>
       <c r="X9" s="68"/>
     </row>
-    <row r="10" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:32" s="51" customFormat="1">
       <c r="B10" s="56"/>
       <c r="C10" s="56"/>
       <c r="D10" s="57"/>
-      <c r="I10" s="116" t="s">
+      <c r="I10" s="119" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-      <c r="T10" s="116"/>
-      <c r="U10" s="116"/>
-      <c r="V10" s="116"/>
-      <c r="W10" s="116"/>
-    </row>
-    <row r="11" spans="1:32" s="51" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="119"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119"/>
+      <c r="T10" s="119"/>
+      <c r="U10" s="119"/>
+      <c r="V10" s="119"/>
+      <c r="W10" s="119"/>
+    </row>
+    <row r="11" spans="1:32" s="51" customFormat="1" ht="27.95" customHeight="1">
       <c r="D11" s="53"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:32">
       <c r="D12" s="53"/>
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
@@ -3022,32 +3022,32 @@
       <c r="V12" s="51"/>
       <c r="W12" s="51"/>
     </row>
-    <row r="13" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C13" s="107" t="s">
+    <row r="13" spans="1:32" ht="20.100000000000001" customHeight="1">
+      <c r="C13" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="107"/>
-      <c r="N13" s="107"/>
-      <c r="O13" s="107"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="107"/>
-      <c r="U13" s="107"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+      <c r="O13" s="120"/>
+      <c r="P13" s="120"/>
+      <c r="Q13" s="120"/>
+      <c r="R13" s="120"/>
+      <c r="S13" s="120"/>
+      <c r="T13" s="120"/>
+      <c r="U13" s="120"/>
       <c r="V13" s="62"/>
       <c r="W13" s="61"/>
     </row>
-    <row r="14" spans="1:32" s="51" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:32" s="51" customFormat="1" ht="12.95" customHeight="1">
       <c r="C14" s="72"/>
       <c r="D14" s="72"/>
       <c r="E14" s="72"/>
@@ -3070,7 +3070,7 @@
       <c r="V14" s="62"/>
       <c r="W14" s="62"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32">
       <c r="B15" s="77"/>
       <c r="C15" s="78"/>
       <c r="D15" s="96"/>
@@ -3095,55 +3095,55 @@
       <c r="W15" s="84"/>
       <c r="X15" s="85"/>
     </row>
-    <row r="16" spans="1:32" s="129" customFormat="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="122"/>
-      <c r="B16" s="126"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="122" t="s">
+    <row r="16" spans="1:32" s="111" customFormat="1" ht="24.75" thickBot="1">
+      <c r="A16" s="104"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="127"/>
-      <c r="F16" s="122" t="s">
+      <c r="E16" s="109"/>
+      <c r="F16" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="122"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="123" t="s">
+      <c r="G16" s="104"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="123"/>
-      <c r="K16" s="123" t="s">
+      <c r="J16" s="105"/>
+      <c r="K16" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123" t="s">
+      <c r="L16" s="105"/>
+      <c r="M16" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
-      <c r="P16" s="123"/>
-      <c r="Q16" s="123"/>
-      <c r="R16" s="123"/>
-      <c r="S16" s="123"/>
-      <c r="T16" s="123"/>
-      <c r="U16" s="123" t="s">
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="105"/>
+      <c r="S16" s="105"/>
+      <c r="T16" s="105"/>
+      <c r="U16" s="105" t="s">
         <v>88</v>
       </c>
-      <c r="V16" s="127"/>
-      <c r="W16" s="123" t="s">
+      <c r="V16" s="109"/>
+      <c r="W16" s="105" t="s">
         <v>89</v>
       </c>
-      <c r="X16" s="128"/>
-      <c r="Y16" s="122"/>
-      <c r="Z16" s="122"/>
-      <c r="AA16" s="122"/>
-      <c r="AB16" s="122"/>
-      <c r="AC16" s="122"/>
-      <c r="AD16" s="122"/>
-      <c r="AE16" s="122"/>
-      <c r="AF16" s="122"/>
-    </row>
-    <row r="17" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="X16" s="110"/>
+      <c r="Y16" s="104"/>
+      <c r="Z16" s="104"/>
+      <c r="AA16" s="104"/>
+      <c r="AB16" s="104"/>
+      <c r="AC16" s="104"/>
+      <c r="AD16" s="104"/>
+      <c r="AE16" s="104"/>
+      <c r="AF16" s="104"/>
+    </row>
+    <row r="17" spans="1:24" ht="19.5" customHeight="1">
       <c r="A17" s="52"/>
       <c r="B17" s="93"/>
       <c r="C17" s="48" t="s">
@@ -3161,41 +3161,41 @@
       <c r="G17" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="111" t="s">
+      <c r="H17" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="109"/>
-      <c r="J17" s="108" t="s">
+      <c r="I17" s="122"/>
+      <c r="J17" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="109"/>
-      <c r="L17" s="108" t="s">
+      <c r="K17" s="122"/>
+      <c r="L17" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="109"/>
-      <c r="N17" s="108" t="s">
+      <c r="M17" s="122"/>
+      <c r="N17" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="O17" s="109"/>
-      <c r="P17" s="108" t="s">
+      <c r="O17" s="122"/>
+      <c r="P17" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="Q17" s="109"/>
-      <c r="R17" s="108" t="s">
+      <c r="Q17" s="122"/>
+      <c r="R17" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="S17" s="109"/>
-      <c r="T17" s="108" t="s">
+      <c r="S17" s="122"/>
+      <c r="T17" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="U17" s="110"/>
-      <c r="V17" s="114" t="s">
+      <c r="U17" s="124"/>
+      <c r="V17" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="W17" s="109"/>
+      <c r="W17" s="122"/>
       <c r="X17" s="86"/>
     </row>
-    <row r="18" spans="1:24" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" ht="14.1" customHeight="1" thickBot="1">
       <c r="A18" s="53"/>
       <c r="B18" s="94"/>
       <c r="C18" s="45" t="s">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="X18" s="88"/>
     </row>
-    <row r="19" spans="1:24" s="51" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" s="51" customFormat="1" ht="23.1" customHeight="1">
       <c r="B19" s="80"/>
       <c r="C19" s="95" t="s">
         <v>71</v>
@@ -3294,64 +3294,64 @@
       <c r="W19" s="90"/>
       <c r="X19" s="91"/>
     </row>
-    <row r="20" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="105" t="s">
+    <row r="20" spans="1:24" s="51" customFormat="1" ht="24">
+      <c r="C20" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="105"/>
-      <c r="E20" s="106" t="s">
+      <c r="D20" s="114"/>
+      <c r="E20" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="106"/>
+      <c r="F20" s="115"/>
       <c r="G20" s="113"/>
-      <c r="I20" s="105" t="s">
+      <c r="I20" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="J20" s="105"/>
-      <c r="K20" s="105"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="105"/>
-      <c r="N20" s="105"/>
-      <c r="O20" s="105"/>
-      <c r="P20" s="105"/>
-      <c r="Q20" s="105"/>
-      <c r="R20" s="105"/>
-      <c r="S20" s="105"/>
-      <c r="T20" s="105"/>
-      <c r="U20" s="105"/>
+      <c r="J20" s="114"/>
+      <c r="K20" s="114"/>
+      <c r="L20" s="114"/>
+      <c r="M20" s="114"/>
+      <c r="N20" s="114"/>
+      <c r="O20" s="114"/>
+      <c r="P20" s="114"/>
+      <c r="Q20" s="114"/>
+      <c r="R20" s="114"/>
+      <c r="S20" s="114"/>
+      <c r="T20" s="114"/>
+      <c r="U20" s="114"/>
       <c r="W20" s="92" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="51" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" s="51" customFormat="1" ht="29.1" customHeight="1">
       <c r="D21" s="53"/>
       <c r="G21" s="113"/>
     </row>
-    <row r="22" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" s="51" customFormat="1">
       <c r="D22" s="53"/>
     </row>
-    <row r="23" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" s="51" customFormat="1">
       <c r="D23" s="53"/>
     </row>
-    <row r="24" spans="1:24" s="51" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C24" s="120" t="s">
+    <row r="24" spans="1:24" s="51" customFormat="1" ht="26.1" customHeight="1">
+      <c r="C24" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="120"/>
-      <c r="E24" s="121" t="s">
+      <c r="D24" s="117"/>
+      <c r="E24" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="121"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="121"/>
-      <c r="K24" s="121"/>
-    </row>
-    <row r="25" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F24" s="118"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="118"/>
+    </row>
+    <row r="25" spans="1:24" s="51" customFormat="1">
       <c r="D25" s="53"/>
     </row>
-    <row r="26" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" s="51" customFormat="1">
       <c r="D26" s="53"/>
       <c r="S26" s="56"/>
       <c r="T26" s="56"/>
@@ -3359,15 +3359,15 @@
       <c r="V26" s="56"/>
       <c r="W26" s="56"/>
     </row>
-    <row r="27" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" s="51" customFormat="1">
       <c r="D27" s="53"/>
       <c r="S27" s="56"/>
       <c r="T27" s="56"/>
-      <c r="U27" s="104"/>
-      <c r="V27" s="104"/>
+      <c r="U27" s="116"/>
+      <c r="V27" s="116"/>
       <c r="W27" s="56"/>
     </row>
-    <row r="28" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" s="51" customFormat="1">
       <c r="D28" s="53"/>
       <c r="S28" s="56"/>
       <c r="T28" s="56"/>
@@ -3375,7 +3375,7 @@
       <c r="V28" s="60"/>
       <c r="W28" s="56"/>
     </row>
-    <row r="29" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" s="51" customFormat="1">
       <c r="D29" s="53"/>
       <c r="S29" s="56"/>
       <c r="T29" s="56"/>
@@ -3383,105 +3383,107 @@
       <c r="V29" s="56"/>
       <c r="W29" s="56"/>
     </row>
-    <row r="30" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" s="51" customFormat="1">
       <c r="D30" s="53"/>
     </row>
-    <row r="31" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" s="51" customFormat="1">
       <c r="D31" s="53"/>
     </row>
-    <row r="32" spans="1:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" s="51" customFormat="1">
       <c r="D32" s="53"/>
     </row>
-    <row r="33" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="4:4" s="51" customFormat="1">
       <c r="D33" s="53"/>
     </row>
-    <row r="34" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:4" s="51" customFormat="1">
       <c r="D34" s="53"/>
     </row>
-    <row r="35" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:4" s="51" customFormat="1">
       <c r="D35" s="53"/>
     </row>
-    <row r="36" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:4" s="51" customFormat="1">
       <c r="D36" s="53"/>
     </row>
-    <row r="37" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:4" s="51" customFormat="1">
       <c r="D37" s="53"/>
     </row>
-    <row r="38" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="4:4" s="51" customFormat="1">
       <c r="D38" s="53"/>
     </row>
-    <row r="39" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:4" s="51" customFormat="1">
       <c r="D39" s="53"/>
     </row>
-    <row r="40" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="4:4" s="51" customFormat="1">
       <c r="D40" s="53"/>
     </row>
-    <row r="41" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="4:4" s="51" customFormat="1">
       <c r="D41" s="53"/>
     </row>
-    <row r="42" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="4:4" s="51" customFormat="1">
       <c r="D42" s="53"/>
     </row>
-    <row r="43" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="4:4" s="51" customFormat="1">
       <c r="D43" s="53"/>
     </row>
-    <row r="44" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="4:4" s="51" customFormat="1">
       <c r="D44" s="53"/>
     </row>
-    <row r="45" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="4:4" s="51" customFormat="1">
       <c r="D45" s="53"/>
     </row>
-    <row r="46" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="4:4" s="51" customFormat="1">
       <c r="D46" s="53"/>
     </row>
-    <row r="47" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:4" s="51" customFormat="1">
       <c r="D47" s="53"/>
     </row>
-    <row r="48" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:4" s="51" customFormat="1">
       <c r="D48" s="53"/>
     </row>
-    <row r="49" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:4" s="51" customFormat="1">
       <c r="D49" s="53"/>
     </row>
-    <row r="50" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="4:4" s="51" customFormat="1">
       <c r="D50" s="53"/>
     </row>
-    <row r="51" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:4" s="51" customFormat="1">
       <c r="D51" s="53"/>
     </row>
-    <row r="52" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:4" s="51" customFormat="1">
       <c r="D52" s="53"/>
     </row>
-    <row r="53" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="4:4" s="51" customFormat="1">
       <c r="D53" s="53"/>
     </row>
-    <row r="54" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:4" s="51" customFormat="1">
       <c r="D54" s="53"/>
     </row>
-    <row r="55" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:4" s="51" customFormat="1">
       <c r="D55" s="53"/>
     </row>
-    <row r="56" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:4" s="51" customFormat="1">
       <c r="D56" s="53"/>
     </row>
-    <row r="57" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:4" s="51" customFormat="1">
       <c r="D57" s="53"/>
     </row>
-    <row r="58" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="4:4" s="51" customFormat="1">
       <c r="D58" s="53"/>
     </row>
-    <row r="59" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="4:4" s="51" customFormat="1">
       <c r="D59" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="I20:U20"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:K24"/>
+    <mergeCell ref="D3:W3"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
     <mergeCell ref="I10:W10"/>
     <mergeCell ref="C13:U13"/>
     <mergeCell ref="H17:I17"/>
@@ -3492,15 +3494,13 @@
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="T17:U17"/>
     <mergeCell ref="V17:W17"/>
-    <mergeCell ref="D3:W3"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I20:U20"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3508,74 +3508,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="2.5" style="51" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="51" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="29" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="51" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="51" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="2.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="2.6640625" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" customWidth="1"/>
-    <col min="20" max="20" width="2.6640625" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" customWidth="1"/>
-    <col min="22" max="22" width="2.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="1.1640625" style="51" customWidth="1"/>
-    <col min="25" max="30" width="10.6640625" style="51" customWidth="1"/>
-    <col min="31" max="32" width="10.83203125" style="51"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="1.140625" style="51" customWidth="1"/>
+    <col min="25" max="30" width="10.7109375" style="51" customWidth="1"/>
+    <col min="31" max="32" width="10.85546875" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" s="51" customFormat="1">
       <c r="D1" s="53"/>
     </row>
-    <row r="2" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:32" s="51" customFormat="1">
       <c r="D2" s="53"/>
     </row>
-    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.15">
-      <c r="D3" s="107" t="s">
+    <row r="3" spans="1:32" ht="18">
+      <c r="D3" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-    </row>
-    <row r="4" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+    </row>
+    <row r="4" spans="1:32" s="51" customFormat="1">
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
       <c r="D4" s="57"/>
@@ -3583,7 +3583,7 @@
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
     </row>
-    <row r="5" spans="1:32" s="51" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" s="51" customFormat="1" ht="13.5" thickBot="1">
       <c r="B5" s="56"/>
       <c r="C5" s="56"/>
       <c r="D5" s="57"/>
@@ -3605,7 +3605,7 @@
       <c r="W5" s="63"/>
       <c r="X5" s="64"/>
     </row>
-    <row r="6" spans="1:32" s="35" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:32" s="35" customFormat="1" ht="20.25" customHeight="1">
       <c r="A6" s="52"/>
       <c r="B6" s="58"/>
       <c r="C6" s="59"/>
@@ -3619,38 +3619,38 @@
       <c r="G6" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="115" t="s">
+      <c r="H6" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="109"/>
-      <c r="J6" s="108" t="s">
+      <c r="I6" s="122"/>
+      <c r="J6" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="109"/>
-      <c r="L6" s="108" t="s">
+      <c r="K6" s="122"/>
+      <c r="L6" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="109"/>
-      <c r="N6" s="108" t="s">
+      <c r="M6" s="122"/>
+      <c r="N6" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="109"/>
-      <c r="P6" s="108" t="s">
+      <c r="O6" s="122"/>
+      <c r="P6" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="108" t="s">
+      <c r="Q6" s="122"/>
+      <c r="R6" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="109"/>
-      <c r="T6" s="108" t="s">
+      <c r="S6" s="122"/>
+      <c r="T6" s="123" t="s">
         <v>50</v>
       </c>
-      <c r="U6" s="109"/>
-      <c r="V6" s="108" t="s">
+      <c r="U6" s="122"/>
+      <c r="V6" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="W6" s="109"/>
+      <c r="W6" s="122"/>
       <c r="X6" s="65"/>
       <c r="Y6" s="52"/>
       <c r="Z6" s="52"/>
@@ -3661,7 +3661,7 @@
       <c r="AE6" s="52"/>
       <c r="AF6" s="52"/>
     </row>
-    <row r="7" spans="1:32" s="29" customFormat="1" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" s="29" customFormat="1" ht="14.1" customHeight="1" thickBot="1">
       <c r="A7" s="53"/>
       <c r="B7" s="57"/>
       <c r="C7" s="60"/>
@@ -3733,7 +3733,7 @@
       <c r="AE7" s="53"/>
       <c r="AF7" s="53"/>
     </row>
-    <row r="8" spans="1:32" s="51" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:32" s="51" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
       <c r="D8" s="57"/>
@@ -3758,32 +3758,32 @@
       <c r="W8" s="67"/>
       <c r="X8" s="68"/>
     </row>
-    <row r="9" spans="1:32" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:32" s="51" customFormat="1">
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
       <c r="D9" s="57"/>
-      <c r="I9" s="116" t="s">
+      <c r="I9" s="119" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-      <c r="T9" s="116"/>
-      <c r="U9" s="116"/>
-      <c r="V9" s="116"/>
-      <c r="W9" s="116"/>
-    </row>
-    <row r="10" spans="1:32" s="51" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
+      <c r="Q9" s="119"/>
+      <c r="R9" s="119"/>
+      <c r="S9" s="119"/>
+      <c r="T9" s="119"/>
+      <c r="U9" s="119"/>
+      <c r="V9" s="119"/>
+      <c r="W9" s="119"/>
+    </row>
+    <row r="10" spans="1:32" s="51" customFormat="1" ht="27.95" customHeight="1">
       <c r="D10" s="53"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:32">
       <c r="D11" s="53"/>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
@@ -3805,32 +3805,32 @@
       <c r="V11" s="51"/>
       <c r="W11" s="51"/>
     </row>
-    <row r="12" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C12" s="107" t="s">
+    <row r="12" spans="1:32" ht="20.100000000000001" customHeight="1">
+      <c r="C12" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="107"/>
-      <c r="K12" s="107"/>
-      <c r="L12" s="107"/>
-      <c r="M12" s="107"/>
-      <c r="N12" s="107"/>
-      <c r="O12" s="107"/>
-      <c r="P12" s="107"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107"/>
-      <c r="U12" s="107"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="120"/>
       <c r="V12" s="62"/>
       <c r="W12" s="61"/>
     </row>
-    <row r="13" spans="1:32" s="51" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:32" s="51" customFormat="1" ht="12.95" customHeight="1">
       <c r="C13" s="72"/>
       <c r="D13" s="72"/>
       <c r="E13" s="72"/>
@@ -3853,7 +3853,7 @@
       <c r="V13" s="62"/>
       <c r="W13" s="62"/>
     </row>
-    <row r="14" spans="1:32" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" ht="13.5" thickBot="1">
       <c r="B14" s="77"/>
       <c r="C14" s="78"/>
       <c r="D14" s="96"/>
@@ -3878,7 +3878,7 @@
       <c r="W14" s="84"/>
       <c r="X14" s="85"/>
     </row>
-    <row r="15" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" ht="19.5" customHeight="1">
       <c r="A15" s="52"/>
       <c r="B15" s="93"/>
       <c r="C15" s="48" t="s">
@@ -3896,41 +3896,41 @@
       <c r="G15" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="111" t="s">
+      <c r="H15" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="109"/>
-      <c r="J15" s="108" t="s">
+      <c r="I15" s="122"/>
+      <c r="J15" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="109"/>
-      <c r="L15" s="108" t="s">
+      <c r="K15" s="122"/>
+      <c r="L15" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="109"/>
-      <c r="N15" s="108" t="s">
+      <c r="M15" s="122"/>
+      <c r="N15" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="O15" s="109"/>
-      <c r="P15" s="108" t="s">
+      <c r="O15" s="122"/>
+      <c r="P15" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="Q15" s="109"/>
-      <c r="R15" s="108" t="s">
+      <c r="Q15" s="122"/>
+      <c r="R15" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="S15" s="109"/>
-      <c r="T15" s="108" t="s">
+      <c r="S15" s="122"/>
+      <c r="T15" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="U15" s="110"/>
-      <c r="V15" s="114" t="s">
+      <c r="U15" s="124"/>
+      <c r="V15" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="W15" s="109"/>
+      <c r="W15" s="122"/>
       <c r="X15" s="86"/>
     </row>
-    <row r="16" spans="1:32" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="14.1" customHeight="1" thickBot="1">
       <c r="A16" s="53"/>
       <c r="B16" s="94"/>
       <c r="C16" s="45" t="s">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="X16" s="88"/>
     </row>
-    <row r="17" spans="2:24" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:24" ht="23.1" customHeight="1">
       <c r="B17" s="80"/>
       <c r="C17" s="95" t="s">
         <v>71</v>
@@ -4029,54 +4029,54 @@
       <c r="W17" s="90"/>
       <c r="X17" s="91"/>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C18" s="105" t="s">
+    <row r="18" spans="2:24" ht="24">
+      <c r="C18" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="105"/>
-      <c r="E18" s="106" t="s">
+      <c r="D18" s="114"/>
+      <c r="E18" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="106"/>
+      <c r="F18" s="115"/>
       <c r="G18" s="113"/>
       <c r="H18" s="51"/>
-      <c r="I18" s="105" t="s">
+      <c r="I18" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
-      <c r="N18" s="105"/>
-      <c r="O18" s="105"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="105"/>
-      <c r="U18" s="105"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="114"/>
+      <c r="L18" s="114"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="114"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="114"/>
+      <c r="Q18" s="114"/>
+      <c r="R18" s="114"/>
+      <c r="S18" s="114"/>
+      <c r="T18" s="114"/>
+      <c r="U18" s="114"/>
       <c r="V18" s="51"/>
       <c r="W18" s="92" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:24" s="51" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:24" s="51" customFormat="1" ht="29.1" customHeight="1">
       <c r="D19" s="53"/>
       <c r="G19" s="113"/>
     </row>
-    <row r="20" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:24" s="51" customFormat="1">
       <c r="D20" s="53"/>
     </row>
-    <row r="21" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:24" s="51" customFormat="1">
       <c r="D21" s="53"/>
     </row>
-    <row r="22" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:24" s="51" customFormat="1">
       <c r="D22" s="53"/>
     </row>
-    <row r="23" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:24" s="51" customFormat="1">
       <c r="D23" s="53"/>
     </row>
-    <row r="24" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:24" s="51" customFormat="1">
       <c r="D24" s="53"/>
       <c r="S24" s="56"/>
       <c r="T24" s="56"/>
@@ -4084,15 +4084,15 @@
       <c r="V24" s="56"/>
       <c r="W24" s="56"/>
     </row>
-    <row r="25" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:24" s="51" customFormat="1">
       <c r="D25" s="53"/>
       <c r="S25" s="56"/>
       <c r="T25" s="56"/>
-      <c r="U25" s="104"/>
-      <c r="V25" s="104"/>
+      <c r="U25" s="116"/>
+      <c r="V25" s="116"/>
       <c r="W25" s="56"/>
     </row>
-    <row r="26" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:24" s="51" customFormat="1">
       <c r="D26" s="53"/>
       <c r="S26" s="56"/>
       <c r="T26" s="56"/>
@@ -4100,7 +4100,7 @@
       <c r="V26" s="60"/>
       <c r="W26" s="56"/>
     </row>
-    <row r="27" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:24" s="51" customFormat="1">
       <c r="D27" s="53"/>
       <c r="S27" s="56"/>
       <c r="T27" s="56"/>
@@ -4108,106 +4108,98 @@
       <c r="V27" s="56"/>
       <c r="W27" s="56"/>
     </row>
-    <row r="28" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:24" s="51" customFormat="1">
       <c r="D28" s="53"/>
     </row>
-    <row r="29" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:24" s="51" customFormat="1">
       <c r="D29" s="53"/>
     </row>
-    <row r="30" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:24" s="51" customFormat="1">
       <c r="D30" s="53"/>
     </row>
-    <row r="31" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:24" s="51" customFormat="1">
       <c r="D31" s="53"/>
     </row>
-    <row r="32" spans="2:24" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:24" s="51" customFormat="1">
       <c r="D32" s="53"/>
     </row>
-    <row r="33" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="4:4" s="51" customFormat="1">
       <c r="D33" s="53"/>
     </row>
-    <row r="34" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:4" s="51" customFormat="1">
       <c r="D34" s="53"/>
     </row>
-    <row r="35" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:4" s="51" customFormat="1">
       <c r="D35" s="53"/>
     </row>
-    <row r="36" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:4" s="51" customFormat="1">
       <c r="D36" s="53"/>
     </row>
-    <row r="37" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:4" s="51" customFormat="1">
       <c r="D37" s="53"/>
     </row>
-    <row r="38" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="4:4" s="51" customFormat="1">
       <c r="D38" s="53"/>
     </row>
-    <row r="39" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:4" s="51" customFormat="1">
       <c r="D39" s="53"/>
     </row>
-    <row r="40" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="4:4" s="51" customFormat="1">
       <c r="D40" s="53"/>
     </row>
-    <row r="41" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="4:4" s="51" customFormat="1">
       <c r="D41" s="53"/>
     </row>
-    <row r="42" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="4:4" s="51" customFormat="1">
       <c r="D42" s="53"/>
     </row>
-    <row r="43" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="4:4" s="51" customFormat="1">
       <c r="D43" s="53"/>
     </row>
-    <row r="44" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="4:4" s="51" customFormat="1">
       <c r="D44" s="53"/>
     </row>
-    <row r="45" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="4:4" s="51" customFormat="1">
       <c r="D45" s="53"/>
     </row>
-    <row r="46" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="4:4" s="51" customFormat="1">
       <c r="D46" s="53"/>
     </row>
-    <row r="47" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:4" s="51" customFormat="1">
       <c r="D47" s="53"/>
     </row>
-    <row r="48" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:4" s="51" customFormat="1">
       <c r="D48" s="53"/>
     </row>
-    <row r="49" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:4" s="51" customFormat="1">
       <c r="D49" s="53"/>
     </row>
-    <row r="50" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="4:4" s="51" customFormat="1">
       <c r="D50" s="53"/>
     </row>
-    <row r="51" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:4" s="51" customFormat="1">
       <c r="D51" s="53"/>
     </row>
-    <row r="52" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:4" s="51" customFormat="1">
       <c r="D52" s="53"/>
     </row>
-    <row r="53" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="4:4" s="51" customFormat="1">
       <c r="D53" s="53"/>
     </row>
-    <row r="54" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:4" s="51" customFormat="1">
       <c r="D54" s="53"/>
     </row>
-    <row r="55" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:4" s="51" customFormat="1">
       <c r="D55" s="53"/>
     </row>
-    <row r="56" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:4" s="51" customFormat="1">
       <c r="D56" s="53"/>
     </row>
-    <row r="57" spans="4:4" s="51" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:4" s="51" customFormat="1">
       <c r="D57" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C12:U12"/>
-    <mergeCell ref="I9:W9"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
     <mergeCell ref="U25:V25"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
@@ -4224,6 +4216,14 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C12:U12"/>
+    <mergeCell ref="I9:W9"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4231,41 +4231,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="256" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="117" t="s">
+    <row r="1" spans="1:256" ht="27.6" customHeight="1">
+      <c r="A1" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-    </row>
-    <row r="2" spans="1:256" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+    </row>
+    <row r="2" spans="1:256" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:256" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:256" ht="32.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:256" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:256" ht="25.5">
       <c r="A4" s="30" t="s">
         <v>48</v>
       </c>
@@ -4565,7 +4565,7 @@
       <c r="IU4" s="28"/>
       <c r="IV4" s="28"/>
     </row>
-    <row r="5" spans="1:256" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:256" ht="32.1" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:256" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:256" ht="31.5" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -4599,18 +4599,18 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:256" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:256" ht="24.95" customHeight="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-    </row>
-    <row r="8" spans="1:256" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+    </row>
+    <row r="8" spans="1:256" ht="32.1" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -4650,7 +4650,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>18</v>
       </c>
@@ -4680,7 +4680,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -4699,7 +4699,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:256" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:256" ht="25.5">
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
@@ -4718,7 +4718,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:256" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:256" ht="20.25" customHeight="1">
       <c r="A14" s="18" t="s">
         <v>41</v>
       </c>
@@ -4737,7 +4737,7 @@
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="1:256" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:256" ht="32.25" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" s="22" t="s">
         <v>25</v>
@@ -4774,8 +4774,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV16"/>
@@ -4787,28 +4787,28 @@
       <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="28" customWidth="1"/>
-    <col min="2" max="3" width="16.33203125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="28" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="28" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" style="28" customWidth="1"/>
-    <col min="7" max="256" width="16.33203125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="28" customWidth="1"/>
+    <col min="2" max="3" width="16.28515625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="28" customWidth="1"/>
+    <col min="7" max="256" width="16.28515625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="117" t="s">
+    <row r="1" spans="1:256" ht="27.6" customHeight="1">
+      <c r="A1" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-    </row>
-    <row r="2" spans="1:256" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+    </row>
+    <row r="2" spans="1:256" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:256" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:256" ht="32.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:256" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:256" ht="25.5">
       <c r="A4" s="30" t="s">
         <v>48</v>
       </c>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="G4" s="32"/>
     </row>
-    <row r="5" spans="1:256" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:256" ht="32.1" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -4872,7 +4872,7 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:256" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:256" ht="42" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -4891,18 +4891,18 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:256" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:256" ht="24.95" customHeight="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="118" t="s">
+      <c r="B7" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-    </row>
-    <row r="8" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+    </row>
+    <row r="8" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -4921,7 +4921,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -4940,7 +4940,7 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:256" s="40" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:256" s="40" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="38" t="s">
         <v>29</v>
       </c>
@@ -5202,7 +5202,7 @@
       <c r="IU10" s="39"/>
       <c r="IV10" s="39"/>
     </row>
-    <row r="11" spans="1:256" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:256" ht="32.1" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>30</v>
       </c>
@@ -5221,7 +5221,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>31</v>
       </c>
@@ -5232,7 +5232,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
@@ -5247,7 +5247,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:256" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:256" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>33</v>
       </c>
@@ -5258,7 +5258,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:256" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:256" ht="20.25" customHeight="1">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
@@ -5267,7 +5267,7 @@
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="1:256" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:256" ht="32.25" customHeight="1">
       <c r="A16" s="21"/>
       <c r="B16" s="22" t="s">
         <v>25</v>

</xml_diff>